<commit_message>
add all benchmarks for SRC2018
</commit_message>
<xml_diff>
--- a/synquid/test/succinct/test_result_overall.xlsx
+++ b/synquid/test/succinct/test_result_overall.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="95">
   <si>
     <t>AVL-BalL0</t>
   </si>
@@ -310,19 +310,7 @@
     <t>synquid</t>
   </si>
   <si>
-    <t>BST-Delete-T2-10</t>
-  </si>
-  <si>
-    <t>BST-Delete-T2-20</t>
-  </si>
-  <si>
-    <t>BST-Delete-T2-30</t>
-  </si>
-  <si>
-    <t>BST-Delete-T2-40</t>
-  </si>
-  <si>
-    <t>BST-Delete-T2-50</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1848,37 +1836,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1908,7 +1866,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -1994,7 +1964,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -2064,6 +2046,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="497723968"/>
         <c:axId val="497721344"/>
@@ -2075,6 +2058,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Depth</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2140,6 +2178,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2184,7 +2277,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3123,37 +3216,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -3198,54 +3261,67 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>compare!$L$41:$L$46</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+            <c:numRef>
+              <c:f>compare!$L$41:$L$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>BST-Delete-T2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BST-Delete-T2-10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>BST-Delete-T2-20</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>BST-Delete-T2-30</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>BST-Delete-T2-40</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>BST-Delete-T2-50</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>compare!$M$41:$M$46</c:f>
+              <c:f>compare!$M$41:$M$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>28.43</c:v>
+                  <c:v>4.5599999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.96</c:v>
+                  <c:v>4.51</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.9</c:v>
+                  <c:v>4.51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.84</c:v>
+                  <c:v>4.47</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.07</c:v>
+                  <c:v>4.68</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.93</c:v>
+                  <c:v>4.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.66</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3253,7 +3329,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-73ED-4761-A95F-5F1ECAF41097}"/>
+              <c16:uniqueId val="{00000000-EB8D-49A6-9DB4-CC814E7AA250}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3296,54 +3372,67 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>compare!$L$41:$L$46</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+            <c:numRef>
+              <c:f>compare!$L$41:$L$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>BST-Delete-T2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BST-Delete-T2-10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>BST-Delete-T2-20</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>BST-Delete-T2-30</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>BST-Delete-T2-40</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>BST-Delete-T2-50</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>compare!$N$41:$N$46</c:f>
+              <c:f>compare!$N$41:$N$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.5599999999999996</c:v>
+                  <c:v>30.21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.51</c:v>
+                  <c:v>31.64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.51</c:v>
+                  <c:v>32.71</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.47</c:v>
+                  <c:v>33.81</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.68</c:v>
+                  <c:v>34.67</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.68</c:v>
+                  <c:v>35.479999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39.39</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48.84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3351,7 +3440,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-73ED-4761-A95F-5F1ECAF41097}"/>
+              <c16:uniqueId val="{00000001-EB8D-49A6-9DB4-CC814E7AA250}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3365,16 +3454,76 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="501368768"/>
-        <c:axId val="501364176"/>
+        <c:axId val="503221136"/>
+        <c:axId val="422147368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="501368768"/>
+        <c:axId val="503221136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>#</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of components</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3412,7 +3561,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="501364176"/>
+        <c:crossAx val="422147368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3420,7 +3569,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="501364176"/>
+        <c:axId val="422147368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3440,6 +3589,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3471,7 +3675,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="501368768"/>
+        <c:crossAx val="503221136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3484,7 +3688,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6346,15 +6550,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>22225</xdr:colOff>
+      <xdr:colOff>15875</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>327025</xdr:colOff>
+      <xdr:colOff>320675</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6454,22 +6658,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>377825</xdr:colOff>
+      <xdr:colOff>523875</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>73025</xdr:colOff>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF0F4E03-F282-42B5-BED4-8DA3525691C6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BAFD2B0-FD32-4550-9FD4-DD4F4C9FFED8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8299,10 +8503,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:V94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="T37" sqref="T37"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8656,7 +8860,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -8667,7 +8871,7 @@
         <v>8.64</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -8678,7 +8882,7 @@
         <v>4.28</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -8689,7 +8893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -8700,7 +8904,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -8711,7 +8915,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -8722,7 +8926,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -8733,7 +8937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -8749,8 +8953,11 @@
       <c r="N40" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="V40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -8760,17 +8967,17 @@
       <c r="C41">
         <v>0.67</v>
       </c>
-      <c r="L41" t="s">
-        <v>19</v>
+      <c r="L41">
+        <v>0</v>
       </c>
       <c r="M41">
-        <v>28.43</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="N41">
-        <v>4.5599999999999996</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+        <v>30.21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -8780,17 +8987,17 @@
       <c r="C42">
         <v>1.1399999999999999</v>
       </c>
-      <c r="L42" t="s">
-        <v>94</v>
+      <c r="L42">
+        <v>10</v>
       </c>
       <c r="M42">
-        <v>29.96</v>
+        <v>4.51</v>
       </c>
       <c r="N42">
-        <v>4.51</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+        <v>31.64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -8800,17 +9007,17 @@
       <c r="C43">
         <v>2.06</v>
       </c>
-      <c r="L43" t="s">
-        <v>95</v>
+      <c r="L43">
+        <v>20</v>
       </c>
       <c r="M43">
-        <v>30.9</v>
+        <v>4.51</v>
       </c>
       <c r="N43">
-        <v>4.51</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+        <v>32.71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -8820,17 +9027,17 @@
       <c r="C44">
         <v>4.12</v>
       </c>
-      <c r="L44" t="s">
-        <v>96</v>
+      <c r="L44">
+        <v>30</v>
       </c>
       <c r="M44">
-        <v>31.84</v>
+        <v>4.47</v>
       </c>
       <c r="N44">
-        <v>4.47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+        <v>33.81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -8840,17 +9047,17 @@
       <c r="C45">
         <v>3.67</v>
       </c>
-      <c r="L45" t="s">
-        <v>97</v>
+      <c r="L45">
+        <v>40</v>
       </c>
       <c r="M45">
-        <v>33.07</v>
+        <v>4.68</v>
       </c>
       <c r="N45">
-        <v>4.68</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+        <v>34.67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -8860,17 +9067,17 @@
       <c r="C46">
         <v>0.61</v>
       </c>
-      <c r="L46" t="s">
-        <v>98</v>
+      <c r="L46">
+        <v>50</v>
       </c>
       <c r="M46">
-        <v>33.93</v>
+        <v>4.68</v>
       </c>
       <c r="N46">
-        <v>4.68</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+        <v>35.479999999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -8880,8 +9087,17 @@
       <c r="C47">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L47">
+        <v>75</v>
+      </c>
+      <c r="M47">
+        <v>4.66</v>
+      </c>
+      <c r="N47">
+        <v>39.39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -8890,6 +9106,15 @@
       </c>
       <c r="C48">
         <v>0.61</v>
+      </c>
+      <c r="L48">
+        <v>100</v>
+      </c>
+      <c r="M48">
+        <v>4.57</v>
+      </c>
+      <c r="N48">
+        <v>48.84</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>